<commit_message>
commit content tai lieu
</commit_message>
<xml_diff>
--- a/vohoangphu.php/structure_page_tai_lieu_php.xlsx
+++ b/vohoangphu.php/structure_page_tai_lieu_php.xlsx
@@ -7,15 +7,17 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="bài tập php" sheetId="4" r:id="rId1"/>
-    <sheet name="tài liệu php" sheetId="3" r:id="rId2"/>
+    <sheet name="mã nguồn mở php" sheetId="6" r:id="rId1"/>
+    <sheet name="công cụ lập trình php" sheetId="5" r:id="rId2"/>
+    <sheet name="bài tập php" sheetId="4" r:id="rId3"/>
+    <sheet name="tài liệu php" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
   <si>
     <t>#</t>
   </si>
@@ -100,6 +102,75 @@
   </si>
   <si>
     <t>strong</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://freetuts.net/hoc-php/bai-tap-php-can-ban" title="Bài tập PHP căn bản có lời giải"&gt; &lt;i class="momizat-icon-star" style="color:#fff;"&gt;&lt;/i&gt; Bài tập PHP căn bản có lời giải &lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Bài tập php</t>
+  </si>
+  <si>
+    <t>tài liệu php</t>
+  </si>
+  <si>
+    <t>công cụ lập trình php</t>
+  </si>
+  <si>
+    <t>&lt;a href="/lap-trinh-web/238-5-ide-tot-nhat-thuong-duoc-su-dung-trong-lap-trinh-php.html" itemprop="url" title="5 IDE tốt nhất thường được sử dụng trong lập trình PHP"&gt; 5 IDE tốt nhất thường được sử dụng trong lập trình PHP&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>5 IDE tốt nhất thường được sử dụng trong lập trình PHP</t>
+  </si>
+  <si>
+    <t>http://hoclaptrinhweb.org/lap-trinh-web/238-5-ide-tot-nhat-thuong-duoc-su-dung-trong-lap-trinh-php.html</t>
+  </si>
+  <si>
+    <t>&lt;a href="/hoc-thiet-ke-web/lap-trinh-web.html"&gt;lập trình PHP&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lập trình PHP</t>
+  </si>
+  <si>
+    <t>&lt;a href="/hoc-thiet-ke-web/lap-trinh-web.html"&gt;Lập trình web PHP &amp;amp; MySQL&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Lập trình web PHP &amp; MySQL</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://netbeans.org/downloads/" target="_blank"&gt;Netbeans&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Netbeans</t>
+  </si>
+  <si>
+    <t>&lt;a href="/component/tags/tag/61-ide-lap-trinh-php.html" class="label label-info"&gt;
+      IDE lập trình php     &lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>IDE lập trình php</t>
+  </si>
+  <si>
+    <t>&lt;a href="/component/tags/tag/62-cong-cu-lap-trinh-php.html" class="label label-info"&gt;
+      công cụ lập trình php     &lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>mã nguồn mở php</t>
+  </si>
+  <si>
+    <t>&lt;a href="/lap-trinh-web/221-3-ma-nguon-mo-dung-de-xay-dung-website-ban-hang-de-dang.html" itemprop="url" title="3 mã nguồn mở dùng để xây dựng website bán hàng dễ dàng"&gt;
+    3 mã nguồn mở dùng để xây dựng website bán hàng dễ dàng&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>3 mã nguồn mở dùng để xây dựng website bán hàng dễ dàng</t>
+  </si>
+  <si>
+    <t>http://hoclaptrinhweb.org/lap-trinh-web/221-3-ma-nguon-mo-dung-de-xay-dung-website-ban-hang-de-dang.html</t>
+  </si>
+  <si>
+    <t>&lt;a href="http://www.opencart.com/" target="_blank"&gt;OpenCart&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>OpenCart</t>
   </si>
 </sst>
 </file>
@@ -530,245 +601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="57.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="52" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="4">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5">
-        <v>2</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="4">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="5">
-        <v>4</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="4">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="5">
-        <v>6</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="4">
-        <v>7</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="5">
-        <v>8</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="4">
-        <v>9</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5">
-        <v>10</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="4">
-        <v>11</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="5">
-        <v>12</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="4">
-        <v>13</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="5">
-        <v>14</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="4">
-        <v>15</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="5">
-        <v>16</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="4">
-        <v>17</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:F4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F22"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -784,7 +617,747 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="8"/>
+      <c r="B3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="5">
+        <v>2</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="5">
+        <v>4</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="5">
+        <v>6</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="5">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="5">
+        <v>10</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <v>11</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="5">
+        <v>12</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
+        <v>13</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="5">
+        <v>14</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="4">
+        <v>15</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="5">
+        <v>16</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="4">
+        <v>17</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:F4"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:F22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="57.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="52" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="5">
+        <v>2</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="5">
+        <v>4</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="5">
+        <v>6</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="5">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="5">
+        <v>10</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <v>11</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="5">
+        <v>12</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
+        <v>13</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="5">
+        <v>14</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="4">
+        <v>15</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="5">
+        <v>16</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="4">
+        <v>17</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:F4"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:F22"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="57.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="52" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="5">
+        <v>2</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="5">
+        <v>4</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="5">
+        <v>6</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="5">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="5">
+        <v>10</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <v>11</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="5">
+        <v>12</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
+        <v>13</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="5">
+        <v>14</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="4">
+        <v>15</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="5">
+        <v>16</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="2:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="4">
+        <v>17</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:F22"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="57.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="52" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>

</xml_diff>